<commit_message>
MSC template update (begin work on facings)
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS_SAND/MSC/Data/MSC Template v1.0.xlsx
+++ b/Projects/CCBOTTLERSUS_SAND/MSC/Data/MSC Template v1.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="71">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -130,10 +130,13 @@
     <t xml:space="preserve">brand</t>
   </si>
   <si>
-    <t xml:space="preserve">Add. Attribute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum count</t>
+    <t xml:space="preserve">att1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">att3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum facings</t>
   </si>
   <si>
     <t xml:space="preserve">Store Type</t>
@@ -148,7 +151,7 @@
     <t xml:space="preserve">COKE CLASSIC</t>
   </si>
   <si>
-    <t xml:space="preserve">SSD MULTI-SERVE,TRANSACTION PACKAGE,SSD IC (att 1)</t>
+    <t xml:space="preserve">SSD MULTI-SERVE,TRANSACTION PACKAGE,SSD IC</t>
   </si>
   <si>
     <t xml:space="preserve">12OZ CANS (att 1)</t>
@@ -166,7 +169,7 @@
     <t xml:space="preserve">FANTA ORANGE,FANTA PINEAPPLE</t>
   </si>
   <si>
-    <t xml:space="preserve">CSD 20oz Flavors (att 3)</t>
+    <t xml:space="preserve">CSD 20oz Flavors</t>
   </si>
   <si>
     <t xml:space="preserve">*No SKU in system: Coca-Cola Orange Vanilla</t>
@@ -184,16 +187,10 @@
     <t xml:space="preserve">GOLD PEAK TEA,HONEST TEA,PEACE TEA,FUZE</t>
   </si>
   <si>
-    <t xml:space="preserve">Group 1 Param</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group 1 Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group 2 Param</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group 2 Value</t>
+    <t xml:space="preserve">Brand Group 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand Group 2</t>
   </si>
   <si>
     <t xml:space="preserve">Group 1 Minimum Facing</t>
@@ -206,9 +203,6 @@
   </si>
   <si>
     <t xml:space="preserve">MONSTER COFFEE+ENERGY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPI_name</t>
   </si>
   <si>
     <t xml:space="preserve">size</t>
@@ -465,8 +459,8 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -474,7 +468,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.6037037037037"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.62222222222222"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.8111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.4962962962963"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="97.7"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.62222222222222"/>
   </cols>
@@ -726,27 +720,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.5111111111111"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9740740740741"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0814814814815"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.3888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="57.4259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.9740740740741"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="57.4259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -759,7 +753,7 @@
       <c r="D1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -768,153 +762,156 @@
       <c r="G1" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H1" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="F5" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="E6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" s="7" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J6" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" s="7" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="F7" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I7" s="7" t="s">
+      <c r="G7" s="8" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J7" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="F8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="F9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>50</v>
+      <c r="G9" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -933,111 +930,83 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.8962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.7407407407407"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="D2" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="0" t="n">
+      <c r="D3" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1055,13 +1024,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.662962962963"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2962962962963"/>
@@ -1069,9 +1038,9 @@
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="34.2962962962963"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>33</v>
@@ -1080,165 +1049,141 @@
         <v>34</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>7.5</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>7.5</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>7.5</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>7.5</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>